<commit_message>
datos testeo y correciones del sistema
</commit_message>
<xml_diff>
--- a/SPRINT 1/CRONOGRAMA VERSUS 3.xlsx
+++ b/SPRINT 1/CRONOGRAMA VERSUS 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73a9b2cc98479d66/Documentos/RESIDENCIA/FarmaciaGiDocumentos/SPRINT 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="309" documentId="8_{64C3392B-9126-40B1-86A9-6A168394F8CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{93D870FF-BDAD-4085-A2FC-F2872D458F26}"/>
+  <xr:revisionPtr revIDLastSave="527" documentId="8_{64C3392B-9126-40B1-86A9-6A168394F8CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DD800CFC-35EC-4195-9ED1-7351FA309E50}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{DD5450A7-52F7-4CDB-9166-D906894400A3}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="571">
   <si>
     <t>Sprint</t>
   </si>
@@ -783,15 +783,6 @@
     <t>El&lt;iminar empleado</t>
   </si>
   <si>
-    <t>cantidad de compra</t>
-  </si>
-  <si>
-    <t>cantidad de venta</t>
-  </si>
-  <si>
-    <t>cantidad de ganancia</t>
-  </si>
-  <si>
     <t>cantidad de inventario por sucursal</t>
   </si>
   <si>
@@ -834,9 +825,6 @@
     <t>borrar detalle en devolucion</t>
   </si>
   <si>
-    <t>PIDIO ASESORA EXTERNA</t>
-  </si>
-  <si>
     <t>agregar rutas  poner url o que parte estamos</t>
   </si>
   <si>
@@ -930,9 +918,6 @@
     <t xml:space="preserve">el cliente se agrego correctamente </t>
   </si>
   <si>
-    <t>paginate de inventario?</t>
-  </si>
-  <si>
     <t>paginar</t>
   </si>
   <si>
@@ -972,9 +957,6 @@
     <t>el administrador no puede seleccionar clientes para verlos</t>
   </si>
   <si>
-    <t>EN EL BUSCADOR DE INVENTARIO QUITAR SUBPRODUCTOS Y OFERTAS</t>
-  </si>
-  <si>
     <t xml:space="preserve">CONFIRMAR EDITAR PRODUCTO </t>
   </si>
   <si>
@@ -1020,12 +1002,6 @@
     <t>inventario rapido</t>
   </si>
   <si>
-    <t>CALCULAR GANACIAS</t>
-  </si>
-  <si>
-    <t>CALCULAR PERDIDAS*</t>
-  </si>
-  <si>
     <t>MONITOREO</t>
   </si>
   <si>
@@ -1164,9 +1140,6 @@
     <t>OFERTAS</t>
   </si>
   <si>
-    <t>NO SE VE NADA EN OFERTA</t>
-  </si>
-  <si>
     <t>CREAR SUCURSAL</t>
   </si>
   <si>
@@ -1179,9 +1152,6 @@
     <t>CONSULTAR SUCURSAL</t>
   </si>
   <si>
-    <t>AGREGAR CONSULTAR EN TODOS</t>
-  </si>
-  <si>
     <t>ALTA SUCURSAL</t>
   </si>
   <si>
@@ -1284,9 +1254,6 @@
     <t>cargar todas las ofertas y todos los subproductos</t>
   </si>
   <si>
-    <t>checar que la eñe se registre bien en la bd tanto en el servidor como local</t>
-  </si>
-  <si>
     <t>{{ url('/puntoVenta/altaSucursal/` + Suc_Inac[t].id + `')}}</t>
   </si>
   <si>
@@ -1338,9 +1305,6 @@
     <t>checar cantidad de ventas al diA CORTE CAJA</t>
   </si>
   <si>
-    <t>SE MUERE EN CORTE DE CAJA</t>
-  </si>
-  <si>
     <t>pedir clave del empleado en los movimientos</t>
   </si>
   <si>
@@ -1368,15 +1332,9 @@
     <t xml:space="preserve">seguimiento del pedido actual </t>
   </si>
   <si>
-    <t>terminar manual de usuario</t>
-  </si>
-  <si>
     <t>CHECAR BIEN EL BUSCADOR DE PRODUCTO</t>
   </si>
   <si>
-    <t>VALIDAR CAMPOS</t>
-  </si>
-  <si>
     <t>MANDAR MENSAJES DE CONFIRMACION</t>
   </si>
   <si>
@@ -1393,9 +1351,6 @@
   </si>
   <si>
     <t>STOCK O INVENTARIO</t>
-  </si>
-  <si>
-    <t>VERIFICAR:</t>
   </si>
   <si>
     <t>REALIZADOS</t>
@@ -1417,9 +1372,6 @@
     <t>imprimir ticket abono deudores.ticket en devolucion</t>
   </si>
   <si>
-    <t>testear vistas punto venta. Modulos testear</t>
-  </si>
-  <si>
     <t>Programar en cierto tiempo los mensajes de confirmacion</t>
   </si>
   <si>
@@ -1495,9 +1447,6 @@
     <t xml:space="preserve">TODAS LAS SUCURSALES. </t>
   </si>
   <si>
-    <t xml:space="preserve">Pagos de paypal. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Cotizaciones. </t>
   </si>
   <si>
@@ -1540,9 +1489,6 @@
     <t>corregir formato de corte de caja</t>
   </si>
   <si>
-    <t>terminar reportes diarios como lo quiere la doctora</t>
-  </si>
-  <si>
     <t>orregir reporte de inventario: solo funciona con salidas</t>
   </si>
   <si>
@@ -1558,9 +1504,6 @@
     <t>darle responsibidad a vistas del ecomerce</t>
   </si>
   <si>
-    <t>impresión directo del ticket</t>
-  </si>
-  <si>
     <t>vistas de seguimiento de pedido</t>
   </si>
   <si>
@@ -1609,12 +1552,6 @@
     <t>tener 10 valores diferentes para las pruebas</t>
   </si>
   <si>
-    <t>** probar una vez cargados nuevos datos</t>
-  </si>
-  <si>
-    <t>AQUÍ</t>
-  </si>
-  <si>
     <t>checar las observaciones que dijo Sorroza del proyecto</t>
   </si>
   <si>
@@ -1627,9 +1564,6 @@
     <t>values(new.codigoArticulo,  new.nombreArticulo, new.precio, now() )</t>
   </si>
   <si>
-    <t>el error de no hay productos aparece despues al crear subproducto</t>
-  </si>
-  <si>
     <t>DATOS PARA TESTEAR SISTEMA</t>
   </si>
   <si>
@@ -1717,9 +1651,6 @@
     <t>65% DE AVANCE</t>
   </si>
   <si>
-    <t>AGREGAR NOMBRE DE SUCURSAL</t>
-  </si>
-  <si>
     <t>cambiar input direccion de sucursal para hacerlo mas ancho</t>
   </si>
   <si>
@@ -1753,7 +1684,79 @@
     <t>corregir existencias de subproductos</t>
   </si>
   <si>
-    <t>imprimir ticket checar</t>
+    <t>agregar iconos en departmentos</t>
+  </si>
+  <si>
+    <t>ACOMODAR BOTON GUARDAR PRODUCTO EN CREAR NUEVO</t>
+  </si>
+  <si>
+    <t>CHECAR COSTO Y PRECIO INV AL BUSCAR PRODUCTO</t>
+  </si>
+  <si>
+    <t>CONFIRMAR ALTA DE PRODUCTO</t>
+  </si>
+  <si>
+    <t>SE TARDA MUCHO SUBPRODUCTO</t>
+  </si>
+  <si>
+    <t>INPUT PIEZAS SOLO ENTEROS SUBPRODUCTOS</t>
+  </si>
+  <si>
+    <t>DESCRIPCION EN OBSERVACION</t>
+  </si>
+  <si>
+    <t>VERIIFICAR BIEN PROCESO DE AGREGAR DE STOCK SUBPROUCTOS</t>
+  </si>
+  <si>
+    <t>CAMBIAR TEXTOS DE EXISTENCIAS DE SUBPRODUCTOS: EXISTENCIA NUEVO</t>
+  </si>
+  <si>
+    <t>EN PROVEEDORES-&gt; DIRECCION AGREGAR TEXT-AREA</t>
+  </si>
+  <si>
+    <t>expandir tabla compras</t>
+  </si>
+  <si>
+    <t>agregar ojito en compra</t>
+  </si>
+  <si>
+    <t>cerrar en modal info adi compras</t>
+  </si>
+  <si>
+    <t>VER CLAVE EN COBRAR VENTA</t>
+  </si>
+  <si>
+    <t>ERRORES CORREGIDOS</t>
+  </si>
+  <si>
+    <t>HACER</t>
+  </si>
+  <si>
+    <t>HACER NO RELEVANTES</t>
+  </si>
+  <si>
+    <t>DOCUMENTACION</t>
+  </si>
+  <si>
+    <t>ECOMMERVE</t>
+  </si>
+  <si>
+    <t>BUSCAR POR TIPOS PRODUCTOS</t>
+  </si>
+  <si>
+    <t>NO ES NECESARIO</t>
+  </si>
+  <si>
+    <t>1)</t>
+  </si>
+  <si>
+    <t>2)</t>
+  </si>
+  <si>
+    <t>checar reporte inv: cant antes, cant. Despues</t>
+  </si>
+  <si>
+    <t>desabilitar boton imprimir</t>
   </si>
 </sst>
 </file>
@@ -3119,611 +3122,611 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="E1" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="E2" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="E3" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E4" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="E5" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E6" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="E7" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
       <c r="E8" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E9" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E10" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="M10" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="E11" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="M11" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="E12" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="M12" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="E13" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="M13" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="E14" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="M14" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="E15" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="M15" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="E16" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="M16" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E17" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="M17" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="E18" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="M18" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="E19" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="M19" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="E20" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="M20" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="E21" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="M21" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="E22" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="M22" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E23" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
       <c r="M23" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="E24" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
       <c r="M24" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="E25" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="M25" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E26" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="M26" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="E27" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
       <c r="M27" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="E28" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
       <c r="M28" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
       <c r="E29" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="M29" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
       <c r="E30" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="M30" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
       <c r="E31" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="M31" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="M32" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="M33" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="M34" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="M35" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="M36" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="M37" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="M38" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
       <c r="M39" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="M40" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="M41" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M44" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M46" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M48" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="49" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M49" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="50" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M50" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M51" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
     </row>
     <row r="52" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M52" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="53" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M53" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
     </row>
     <row r="54" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M54" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M55" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="56" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M56" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
     </row>
     <row r="57" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M57" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M58" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M59" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M60" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M61" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M62" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
     </row>
     <row r="63" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M63" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
     </row>
     <row r="64" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M64" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
     </row>
     <row r="65" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M65" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
     </row>
     <row r="66" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M66" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
     </row>
     <row r="67" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M67" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
     </row>
     <row r="68" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M68" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
     </row>
     <row r="69" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M69" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="70" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M70" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
     </row>
     <row r="71" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M71" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
     </row>
     <row r="72" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M72" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="73" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M73" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M74" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
     </row>
     <row r="75" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M75" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="76" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M76" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="77" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M77" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="78" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M78" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="79" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M79" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="80" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M80" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
     </row>
     <row r="81" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M81" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="82" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M82" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="83" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M83" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
     </row>
     <row r="84" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M84" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -6825,7 +6828,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>529</v>
+        <v>507</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -6929,36 +6932,48 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389771CD-3F00-45C6-928B-7954571D8EB7}">
-  <dimension ref="A1:O201"/>
+  <dimension ref="A1:Q201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="E14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
     <col min="3" max="3" width="8.42578125" customWidth="1"/>
     <col min="5" max="5" width="49.42578125" customWidth="1"/>
+    <col min="9" max="9" width="16.5703125" customWidth="1"/>
     <col min="13" max="13" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>450</v>
-      </c>
+      <c r="A1" s="26"/>
       <c r="M1" t="s">
-        <v>451</v>
+        <v>436</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>563</v>
+      </c>
+      <c r="D2" t="s">
+        <v>562</v>
+      </c>
       <c r="M2" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>443</v>
+        <v>482</v>
+      </c>
+      <c r="D3" t="s">
+        <v>405</v>
+      </c>
+      <c r="F3" t="s">
+        <v>561</v>
       </c>
       <c r="M3" t="s">
         <v>221</v>
@@ -6972,7 +6987,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>448</v>
+        <v>483</v>
+      </c>
+      <c r="D4" t="s">
+        <v>441</v>
       </c>
       <c r="M4" t="s">
         <v>225</v>
@@ -6985,8 +7003,14 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>484</v>
+      </c>
       <c r="D5" t="s">
-        <v>416</v>
+        <v>434</v>
+      </c>
+      <c r="F5" t="s">
+        <v>406</v>
       </c>
       <c r="M5" t="s">
         <v>226</v>
@@ -7000,7 +7024,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
-        <v>456</v>
+        <v>420</v>
+      </c>
+      <c r="F6" t="s">
+        <v>422</v>
       </c>
       <c r="M6" t="s">
         <v>227</v>
@@ -7013,11 +7040,11 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>417</v>
-      </c>
       <c r="D7" t="s">
-        <v>434</v>
+        <v>442</v>
+      </c>
+      <c r="F7" t="s">
+        <v>400</v>
       </c>
       <c r="M7" t="s">
         <v>235</v>
@@ -7027,11 +7054,11 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>425</v>
-      </c>
       <c r="D8" t="s">
-        <v>436</v>
+        <v>414</v>
+      </c>
+      <c r="F8" t="s">
+        <v>308</v>
       </c>
       <c r="M8" t="s">
         <v>231</v>
@@ -7041,11 +7068,8 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>431</v>
-      </c>
       <c r="D9" t="s">
-        <v>439</v>
+        <v>520</v>
       </c>
       <c r="M9" t="s">
         <v>222</v>
@@ -7055,22 +7079,19 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>432</v>
-      </c>
       <c r="D10" t="s">
-        <v>314</v>
+        <v>565</v>
+      </c>
+      <c r="F10" t="s">
+        <v>294</v>
       </c>
       <c r="M10" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>433</v>
-      </c>
       <c r="D11" t="s">
-        <v>458</v>
+        <v>549</v>
       </c>
       <c r="M11" t="s">
         <v>228</v>
@@ -7080,13 +7101,25 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>540</v>
+      </c>
+      <c r="E12" t="s">
+        <v>564</v>
+      </c>
       <c r="M12" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>493</v>
+        <v>537</v>
+      </c>
+      <c r="E13" t="s">
+        <v>467</v>
+      </c>
+      <c r="F13" t="s">
+        <v>568</v>
       </c>
       <c r="M13" t="s">
         <v>230</v>
@@ -7096,404 +7129,291 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>437</v>
-      </c>
       <c r="D14" t="s">
-        <v>494</v>
+        <v>514</v>
+      </c>
+      <c r="E14" t="s">
+        <v>468</v>
+      </c>
+      <c r="F14" t="s">
+        <v>500</v>
       </c>
       <c r="M14" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>515</v>
+      </c>
+      <c r="E15" t="s">
+        <v>469</v>
+      </c>
+      <c r="F15" t="s">
+        <v>298</v>
+      </c>
       <c r="M15" t="s">
         <v>233</v>
       </c>
       <c r="O15" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>440</v>
+      <c r="D16" t="s">
+        <v>517</v>
+      </c>
+      <c r="E16" t="s">
+        <v>461</v>
+      </c>
+      <c r="F16" t="s">
+        <v>300</v>
       </c>
       <c r="M16" t="s">
         <v>234</v>
       </c>
       <c r="O16" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>325</v>
-      </c>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>495</v>
+        <v>541</v>
+      </c>
+      <c r="E17" t="s">
+        <v>462</v>
       </c>
       <c r="M17" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>326</v>
-      </c>
-      <c r="D18" t="s">
-        <v>496</v>
-      </c>
-      <c r="F18" t="s">
-        <v>521</v>
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>463</v>
       </c>
       <c r="M18" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>464</v>
+      </c>
+      <c r="F19" t="s">
+        <v>567</v>
+      </c>
+      <c r="M19" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>465</v>
+      </c>
+      <c r="F20" t="s">
+        <v>319</v>
+      </c>
+      <c r="M20" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>466</v>
+      </c>
+      <c r="F21" t="s">
+        <v>320</v>
+      </c>
+      <c r="M21" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>424</v>
+      </c>
+      <c r="F22" t="s">
+        <v>321</v>
+      </c>
+      <c r="M22" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>427</v>
+      </c>
+      <c r="F23" t="s">
+        <v>423</v>
+      </c>
+      <c r="M23" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>351</v>
-      </c>
-      <c r="D19" t="s">
-        <v>497</v>
-      </c>
-      <c r="M19" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>373</v>
-      </c>
-      <c r="D20" t="s">
-        <v>499</v>
-      </c>
-      <c r="M20" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>410</v>
-      </c>
-      <c r="D21" t="s">
+    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>428</v>
+      </c>
+      <c r="F24" t="s">
         <v>498</v>
       </c>
-      <c r="F21" t="s">
-        <v>522</v>
-      </c>
-      <c r="M21" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>413</v>
-      </c>
-      <c r="D22" t="s">
-        <v>500</v>
-      </c>
-      <c r="F22" t="s">
-        <v>522</v>
-      </c>
-      <c r="M22" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>435</v>
-      </c>
-      <c r="D23" t="s">
-        <v>501</v>
-      </c>
-      <c r="F23" t="s">
-        <v>522</v>
-      </c>
-      <c r="M23" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>327</v>
-      </c>
-      <c r="D24" t="s">
-        <v>502</v>
-      </c>
-      <c r="F24" t="s">
-        <v>522</v>
-      </c>
       <c r="M24" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>328</v>
-      </c>
-      <c r="D25" t="s">
-        <v>504</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>486</v>
       </c>
       <c r="M25" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>329</v>
-      </c>
-      <c r="D26" t="s">
-        <v>503</v>
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>487</v>
+      </c>
+      <c r="F26" t="s">
+        <v>569</v>
       </c>
       <c r="M26" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>378</v>
-      </c>
-      <c r="D27" t="s">
-        <v>519</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>488</v>
+      </c>
+      <c r="F27" t="s">
+        <v>570</v>
       </c>
       <c r="M27" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>263</v>
-      </c>
-      <c r="D28" t="s">
-        <v>505</v>
-      </c>
+    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>489</v>
+      </c>
+      <c r="F28" s="23"/>
       <c r="M28" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="29" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>497</v>
+      </c>
+      <c r="F29" s="23"/>
+      <c r="M29" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="30" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>485</v>
+      </c>
+      <c r="F30" s="23"/>
+      <c r="M30" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>246</v>
-      </c>
-      <c r="D29" t="s">
-        <v>506</v>
-      </c>
-      <c r="M29" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="23" t="s">
-        <v>247</v>
-      </c>
-      <c r="D30" t="s">
-        <v>507</v>
-      </c>
-      <c r="M30" t="s">
+    <row r="31" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="32" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
-        <v>248</v>
-      </c>
-      <c r="D31" t="s">
-        <v>508</v>
-      </c>
-      <c r="M31" t="s">
+    <row r="39" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="23" t="s">
-        <v>230</v>
-      </c>
-      <c r="D32" t="s">
-        <v>516</v>
-      </c>
-      <c r="M32" t="s">
+    <row r="40" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>291</v>
-      </c>
-      <c r="D33" t="s">
-        <v>517</v>
-      </c>
-      <c r="M33" t="s">
+    <row r="41" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>457</v>
-      </c>
-      <c r="D34" t="s">
-        <v>518</v>
-      </c>
-      <c r="M34" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>441</v>
-      </c>
-      <c r="D35" t="s">
-        <v>520</v>
-      </c>
-      <c r="M35" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>295</v>
-      </c>
-      <c r="D36" t="s">
-        <v>523</v>
-      </c>
-      <c r="M36" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>299</v>
-      </c>
-      <c r="M37" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>303</v>
-      </c>
-      <c r="D38" t="s">
-        <v>524</v>
-      </c>
-      <c r="M38" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>305</v>
-      </c>
-      <c r="D39" t="s">
-        <v>525</v>
-      </c>
-      <c r="M39" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>509</v>
-      </c>
-      <c r="D40" t="s">
-        <v>526</v>
-      </c>
-      <c r="M40" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>510</v>
-      </c>
-      <c r="M41" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>511</v>
-      </c>
-      <c r="D42" t="s">
-        <v>527</v>
-      </c>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M42" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>512</v>
-      </c>
+        <v>280</v>
+      </c>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M43" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="4:13" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
         <v>513</v>
-      </c>
-      <c r="D44" t="s">
-        <v>535</v>
       </c>
       <c r="M44" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>9512861203</v>
-      </c>
-      <c r="D45" t="s">
-        <v>542</v>
-      </c>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M45" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>514</v>
-      </c>
-      <c r="D46" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>515</v>
-      </c>
-      <c r="D47" t="s">
-        <v>537</v>
-      </c>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D48" t="s">
-        <v>539</v>
-      </c>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.25">
       <c r="M48" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>477</v>
-      </c>
-      <c r="D49" t="s">
-        <v>540</v>
-      </c>
       <c r="M49" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>478</v>
-      </c>
-      <c r="D50" t="s">
-        <v>543</v>
+        <v>490</v>
       </c>
       <c r="M50" t="s">
         <v>207</v>
@@ -7501,18 +7421,12 @@
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>479</v>
-      </c>
-      <c r="D51" t="s">
-        <v>541</v>
+        <v>491</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>480</v>
-      </c>
-      <c r="D52" t="s">
-        <v>544</v>
+        <v>492</v>
       </c>
       <c r="M52" t="s">
         <v>208</v>
@@ -7520,10 +7434,7 @@
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>481</v>
-      </c>
-      <c r="D53" t="s">
-        <v>549</v>
+        <v>493</v>
       </c>
       <c r="M53" t="s">
         <v>209</v>
@@ -7531,21 +7442,15 @@
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>482</v>
-      </c>
-      <c r="D54" t="s">
-        <v>557</v>
+        <v>494</v>
       </c>
       <c r="M54" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>483</v>
-      </c>
-      <c r="D55" t="s">
-        <v>558</v>
+      <c r="A55">
+        <v>9512861203</v>
       </c>
       <c r="M55" t="s">
         <v>211</v>
@@ -7553,10 +7458,7 @@
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>484</v>
-      </c>
-      <c r="D56" t="s">
-        <v>559</v>
+        <v>495</v>
       </c>
       <c r="M56" t="s">
         <v>212</v>
@@ -7564,48 +7466,28 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>485</v>
+        <v>496</v>
       </c>
       <c r="B57" t="s">
-        <v>360</v>
-      </c>
-      <c r="D57" t="s">
-        <v>560</v>
+        <v>352</v>
       </c>
       <c r="M57" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D58" t="s">
-        <v>561</v>
-      </c>
-    </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>486</v>
-      </c>
-      <c r="D59" t="s">
-        <v>562</v>
-      </c>
       <c r="M59" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D60" t="s">
-        <v>563</v>
-      </c>
       <c r="M60" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>487</v>
-      </c>
-      <c r="D61" t="s">
-        <v>564</v>
+        <v>470</v>
       </c>
       <c r="M61" t="s">
         <v>205</v>
@@ -7613,10 +7495,7 @@
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>488</v>
-      </c>
-      <c r="D62" t="s">
-        <v>565</v>
+        <v>471</v>
       </c>
       <c r="M62" t="s">
         <v>206</v>
@@ -7624,13 +7503,10 @@
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>489</v>
+        <v>472</v>
       </c>
       <c r="B63" t="s">
-        <v>369</v>
-      </c>
-      <c r="D63" t="s">
-        <v>566</v>
+        <v>361</v>
       </c>
       <c r="M63" t="s">
         <v>207</v>
@@ -7638,10 +7514,7 @@
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>490</v>
-      </c>
-      <c r="D64" t="s">
-        <v>567</v>
+        <v>473</v>
       </c>
       <c r="M64" t="s">
         <v>208</v>
@@ -7649,10 +7522,7 @@
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>383</v>
-      </c>
-      <c r="D65" t="s">
-        <v>568</v>
+        <v>373</v>
       </c>
       <c r="M65" t="s">
         <v>209</v>
@@ -7660,10 +7530,7 @@
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>491</v>
-      </c>
-      <c r="D66" t="s">
-        <v>569</v>
+        <v>474</v>
       </c>
       <c r="M66" t="s">
         <v>210</v>
@@ -7671,7 +7538,7 @@
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="M67" t="s">
         <v>211</v>
@@ -7684,7 +7551,7 @@
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>459</v>
+        <v>443</v>
       </c>
       <c r="M69" t="s">
         <v>213</v>
@@ -7692,7 +7559,7 @@
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="M70" t="s">
         <v>214</v>
@@ -7705,7 +7572,7 @@
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>309</v>
+        <v>503</v>
       </c>
       <c r="M72" t="s">
         <v>225</v>
@@ -7713,45 +7580,48 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>287</v>
+        <v>504</v>
       </c>
       <c r="M73" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>505</v>
+      </c>
       <c r="M74" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M75" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M76" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M77" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M78" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="M80" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="81" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M81" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="82" spans="13:13" x14ac:dyDescent="0.25">
@@ -7761,17 +7631,17 @@
     </row>
     <row r="83" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M83" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="84" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M84" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="85" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M85" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="86" spans="13:13" x14ac:dyDescent="0.25">
@@ -7781,137 +7651,137 @@
     </row>
     <row r="87" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M87" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="88" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M88" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="89" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M89" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="90" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M90" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="91" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M91" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="92" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M92" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="93" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M93" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="94" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M94" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="95" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M95" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="96" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M96" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M97" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="98" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M98" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M99" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="100" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M100" t="s">
-        <v>445</v>
+        <v>431</v>
       </c>
     </row>
     <row r="101" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M101" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
     </row>
     <row r="102" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M102" t="s">
-        <v>449</v>
+        <v>435</v>
       </c>
     </row>
     <row r="103" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M103" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
     </row>
     <row r="104" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M104" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
     </row>
     <row r="105" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M105" t="s">
-        <v>423</v>
+        <v>412</v>
       </c>
     </row>
     <row r="106" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M106" t="s">
-        <v>405</v>
+        <v>395</v>
       </c>
     </row>
     <row r="107" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M107" t="s">
-        <v>406</v>
+        <v>396</v>
       </c>
     </row>
     <row r="108" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M108" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
     </row>
     <row r="109" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M109" t="s">
-        <v>409</v>
+        <v>399</v>
       </c>
     </row>
     <row r="110" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M110" t="s">
-        <v>411</v>
+        <v>401</v>
       </c>
     </row>
     <row r="111" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M111" t="s">
-        <v>412</v>
+        <v>402</v>
       </c>
     </row>
     <row r="112" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M112" t="s">
-        <v>415</v>
+        <v>404</v>
       </c>
     </row>
     <row r="113" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M113" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="114" spans="13:13" x14ac:dyDescent="0.25">
@@ -7921,217 +7791,520 @@
     </row>
     <row r="115" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M115" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
     </row>
     <row r="116" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M116" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
     </row>
     <row r="117" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M117" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
     </row>
     <row r="118" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M118" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="119" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M119" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
     </row>
     <row r="120" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M120" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
     </row>
     <row r="121" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M121" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
     </row>
     <row r="123" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M123" t="s">
-        <v>438</v>
+        <v>426</v>
       </c>
     </row>
     <row r="124" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M124" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
     </row>
     <row r="125" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M125" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="126" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M126" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="127" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M127" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="128" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M128" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
     </row>
     <row r="129" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M129" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
     </row>
     <row r="130" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M130" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="131" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M131" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
     </row>
     <row r="132" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M132" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
     </row>
     <row r="133" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M133" t="s">
-        <v>310</v>
+        <v>304</v>
       </c>
     </row>
     <row r="134" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M134" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="135" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M135" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="136" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M136" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
     </row>
     <row r="137" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M137" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="138" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M138" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="139" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M139" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="140" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M140" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
     </row>
     <row r="141" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M141" s="27" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="142" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M142" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="143" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M143" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="144" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M144" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="145" spans="13:13" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="145" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M145" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="186" spans="2:2" x14ac:dyDescent="0.25">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="146" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M146" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="147" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M147" t="s">
+        <v>241</v>
+      </c>
+      <c r="N147" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="148" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M148" t="s">
+        <v>224</v>
+      </c>
+      <c r="N148" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="149" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M149" t="s">
+        <v>224</v>
+      </c>
+      <c r="N149" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="150" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M150" t="s">
+        <v>224</v>
+      </c>
+      <c r="N150" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="151" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M151" t="s">
+        <v>224</v>
+      </c>
+      <c r="N151" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="152" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M152" t="s">
+        <v>224</v>
+      </c>
+      <c r="N152" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="153" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M153" t="s">
+        <v>241</v>
+      </c>
+      <c r="N153" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="154" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M154" t="s">
+        <v>241</v>
+      </c>
+      <c r="N154" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="155" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M155" t="s">
+        <v>241</v>
+      </c>
+      <c r="N155" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="156" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M156" t="s">
+        <v>224</v>
+      </c>
+      <c r="N156" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="157" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M157" t="s">
+        <v>224</v>
+      </c>
+      <c r="N157" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="158" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M158" t="s">
+        <v>224</v>
+      </c>
+      <c r="N158" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="159" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M159" t="s">
+        <v>241</v>
+      </c>
+      <c r="N159" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="160" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M160" t="s">
+        <v>224</v>
+      </c>
+      <c r="N160" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="161" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M161" t="s">
+        <v>224</v>
+      </c>
+      <c r="N161" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="162" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M162" t="s">
+        <v>224</v>
+      </c>
+      <c r="N162" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="163" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M163" t="s">
+        <v>224</v>
+      </c>
+      <c r="N163" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="164" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M164" t="s">
+        <v>241</v>
+      </c>
+      <c r="N164" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="165" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M165" t="s">
+        <v>241</v>
+      </c>
+      <c r="N165" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="166" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M166" t="s">
+        <v>241</v>
+      </c>
+      <c r="N166" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="167" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M167" t="s">
+        <v>241</v>
+      </c>
+      <c r="N167" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="168" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M168" t="s">
+        <v>287</v>
+      </c>
+      <c r="N168" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="169" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M169" t="s">
+        <v>421</v>
+      </c>
+      <c r="N169" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="170" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M170" t="s">
+        <v>425</v>
+      </c>
+      <c r="N170" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="171" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M171" t="s">
+        <v>224</v>
+      </c>
+      <c r="N171" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="172" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M172" t="s">
+        <v>224</v>
+      </c>
+      <c r="N172" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="173" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M173" t="s">
+        <v>224</v>
+      </c>
+      <c r="N173" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="174" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M174" t="s">
+        <v>224</v>
+      </c>
+      <c r="N174" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="175" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M175" t="s">
+        <v>224</v>
+      </c>
+      <c r="N175" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="176" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M176" t="s">
+        <v>224</v>
+      </c>
+      <c r="N176" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="177" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M177" t="s">
+        <v>224</v>
+      </c>
+      <c r="N177" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="178" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M178" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="179" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M179" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="181" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M181" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="182" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M182" t="s">
+        <v>559</v>
+      </c>
+      <c r="P182" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="183" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M183" t="s">
+        <v>527</v>
+      </c>
+      <c r="Q183" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="184" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M184" t="s">
+        <v>542</v>
+      </c>
+      <c r="P184" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="185" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="M185" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="186" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B186" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="187" spans="2:2" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+      <c r="M186" t="s">
+        <v>343</v>
+      </c>
+      <c r="O186" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="187" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="188" spans="2:2" x14ac:dyDescent="0.25">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="188" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B188" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="189" spans="2:2" x14ac:dyDescent="0.25">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="189" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="190" spans="2:2" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="190" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B190" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="192" spans="2:2" x14ac:dyDescent="0.25">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="192" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B192" t="s">
-        <v>419</v>
+        <v>408</v>
       </c>
     </row>
     <row r="195" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B195" t="s">
-        <v>420</v>
+        <v>409</v>
       </c>
     </row>
     <row r="196" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B196" t="s">
-        <v>421</v>
+        <v>410</v>
       </c>
     </row>
     <row r="197" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
     </row>
     <row r="198" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B198" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
     </row>
     <row r="199" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
-        <v>453</v>
+        <v>438</v>
       </c>
     </row>
     <row r="200" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
-        <v>455</v>
+        <v>440</v>
       </c>
     </row>
     <row r="201" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
-        <v>452</v>
+        <v>437</v>
       </c>
     </row>
   </sheetData>
@@ -8160,7 +8333,7 @@
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>528</v>
+        <v>506</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -8169,7 +8342,7 @@
         <v>199</v>
       </c>
       <c r="C4" t="s">
-        <v>538</v>
+        <v>516</v>
       </c>
       <c r="D4" t="s">
         <v>200</v>
@@ -8190,21 +8363,21 @@
         <v>224</v>
       </c>
       <c r="D7" t="s">
-        <v>547</v>
+        <v>525</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="31"/>
       <c r="D8" t="s">
-        <v>548</v>
+        <v>526</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="30" t="s">
-        <v>529</v>
+        <v>507</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8212,7 +8385,7 @@
         <v>224</v>
       </c>
       <c r="D10" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8221,7 +8394,7 @@
         <v>224</v>
       </c>
       <c r="D11" t="s">
-        <v>531</v>
+        <v>509</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8230,7 +8403,7 @@
         <v>224</v>
       </c>
       <c r="D12" t="s">
-        <v>553</v>
+        <v>531</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -8239,7 +8412,7 @@
         <v>224</v>
       </c>
       <c r="D13" t="s">
-        <v>533</v>
+        <v>511</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -8248,7 +8421,7 @@
         <v>224</v>
       </c>
       <c r="D14" t="s">
-        <v>532</v>
+        <v>510</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -8257,7 +8430,7 @@
         <v>224</v>
       </c>
       <c r="D15" t="s">
-        <v>554</v>
+        <v>532</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -8266,7 +8439,7 @@
         <v>224</v>
       </c>
       <c r="D16" t="s">
-        <v>545</v>
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -8274,7 +8447,7 @@
       <c r="B17" s="30"/>
       <c r="C17" s="23"/>
       <c r="D17" t="s">
-        <v>555</v>
+        <v>533</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -8289,7 +8462,7 @@
         <v>241</v>
       </c>
       <c r="D19" t="s">
-        <v>534</v>
+        <v>512</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -8298,7 +8471,7 @@
         <v>241</v>
       </c>
       <c r="D20" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -8307,7 +8480,7 @@
         <v>241</v>
       </c>
       <c r="D21" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -8316,7 +8489,7 @@
         <v>241</v>
       </c>
       <c r="D22" t="s">
-        <v>546</v>
+        <v>524</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -8325,7 +8498,7 @@
         <v>241</v>
       </c>
       <c r="D23" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -8337,31 +8510,31 @@
         <v>181</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" s="30"/>
       <c r="D26" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="30"/>
       <c r="D27" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="30"/>
       <c r="D28" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="30"/>
       <c r="D29" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -8370,55 +8543,55 @@
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="30"/>
       <c r="D31" s="30" t="s">
-        <v>530</v>
+        <v>508</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="30"/>
       <c r="D32" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" s="30"/>
       <c r="D33" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="30"/>
       <c r="D34" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="30"/>
       <c r="D35" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B36" s="30"/>
       <c r="D36" t="s">
-        <v>364</v>
+        <v>356</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="30"/>
       <c r="D37" t="s">
-        <v>402</v>
+        <v>392</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="30"/>
       <c r="D38" t="s">
-        <v>365</v>
+        <v>357</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="30"/>
       <c r="D39" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -8427,50 +8600,50 @@
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="30"/>
       <c r="D41" s="30" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
       <c r="D42" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
       <c r="D43" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B44" s="30"/>
       <c r="D44" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="31"/>
       <c r="D45" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="31"/>
       <c r="D46" t="s">
-        <v>404</v>
+        <v>394</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="31"/>
       <c r="D47" s="30" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="31"/>
       <c r="D48" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -8484,7 +8657,7 @@
         <v>241</v>
       </c>
       <c r="D50" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -8493,7 +8666,7 @@
         <v>241</v>
       </c>
       <c r="D51" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -8502,7 +8675,7 @@
         <v>241</v>
       </c>
       <c r="D52" t="s">
-        <v>400</v>
+        <v>390</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -8511,7 +8684,7 @@
         <v>241</v>
       </c>
       <c r="D53" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -8523,56 +8696,56 @@
         <v>193</v>
       </c>
       <c r="D55" s="30" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="30"/>
       <c r="B56" s="30"/>
       <c r="D56" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="30"/>
       <c r="B57" s="30"/>
       <c r="D57" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="30"/>
       <c r="B58" s="30"/>
       <c r="D58" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="30"/>
       <c r="B59" s="30"/>
       <c r="D59" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="30"/>
       <c r="B60" s="30"/>
       <c r="D60" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="30"/>
       <c r="B61" s="30"/>
       <c r="D61" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="30"/>
       <c r="B62" s="30"/>
       <c r="D62" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -8583,13 +8756,13 @@
         <v>197</v>
       </c>
       <c r="D64" t="s">
-        <v>550</v>
+        <v>528</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="30"/>
       <c r="D65" t="s">
-        <v>551</v>
+        <v>529</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
@@ -8600,19 +8773,19 @@
         <v>186</v>
       </c>
       <c r="D67" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B68" s="30"/>
       <c r="D68" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B69" s="30"/>
       <c r="D69" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.25">
@@ -8623,13 +8796,13 @@
         <v>195</v>
       </c>
       <c r="D71" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B72" s="30"/>
       <c r="D72" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.25">
@@ -8640,13 +8813,13 @@
         <v>188</v>
       </c>
       <c r="D74" s="30" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B75" s="30"/>
       <c r="D75" s="30" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.25">
@@ -8662,31 +8835,31 @@
         <v>187</v>
       </c>
       <c r="D78" s="30" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B79" s="30"/>
       <c r="D79" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B80" s="30"/>
       <c r="D80" t="s">
-        <v>552</v>
+        <v>530</v>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B81" s="30"/>
       <c r="D81" t="s">
-        <v>395</v>
+        <v>385</v>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B82" s="31"/>
       <c r="D82" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.25">
@@ -8698,7 +8871,7 @@
       </c>
       <c r="C84" s="23"/>
       <c r="D84" t="s">
-        <v>556</v>
+        <v>534</v>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.25">
@@ -8756,42 +8929,42 @@
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="30" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>392</v>
+        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>393</v>
+        <v>383</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="139" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="I139" s="26" t="s">
-        <v>454</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modificaciones en el sistema
</commit_message>
<xml_diff>
--- a/SPRINT 1/CRONOGRAMA VERSUS 3.xlsx
+++ b/SPRINT 1/CRONOGRAMA VERSUS 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73a9b2cc98479d66/Documentos/RESIDENCIA/FarmaciaGiDocumentos/SPRINT 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="586" documentId="8_{64C3392B-9126-40B1-86A9-6A168394F8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58C8A696-51E2-4EEB-9940-007ED93040EE}"/>
+  <xr:revisionPtr revIDLastSave="637" documentId="8_{64C3392B-9126-40B1-86A9-6A168394F8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC166B56-EC77-48BE-A26C-35C9BA16CA94}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="7" xr2:uid="{DD5450A7-52F7-4CDB-9166-D906894400A3}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1139" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="619">
   <si>
     <t>Sprint</t>
   </si>
@@ -1853,6 +1853,54 @@
   </si>
   <si>
     <t>en buscar venta registrar en la col pago que se lleva pagando en esa venta a creditoporque solo mantiene 0 hasta liquidar marca completo en esa col</t>
+  </si>
+  <si>
+    <t>validar cuando no hay clientes</t>
+  </si>
+  <si>
+    <t>verificar si en buscar productos no busca los subproductos</t>
+  </si>
+  <si>
+    <t>clientes numero negativo en telefono</t>
+  </si>
+  <si>
+    <t>$users = DB::table('users')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            -&gt;join('contacts', 'users.id', '=', 'contacts.user_id')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            -&gt;join('orders', 'users.id', '=', 'orders.user_id')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            -&gt;select('users.*', 'contacts.phone', 'orders.price')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            -&gt;get();</t>
+  </si>
+  <si>
+    <t>DB::table('users')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        -&gt;join('contacts', function ($join) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            $join-&gt;on('users.id', '=', 'contacts.user_id')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                 -&gt;where('contacts.user_id', '&gt;', 5);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        })</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        -&gt;get();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agregar mensaje y </t>
+  </si>
+  <si>
+    <t>OPTIMIZAR CODIGO BUSCAR VENTA EN DEVOLUCION</t>
   </si>
 </sst>
 </file>
@@ -7030,7 +7078,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{389771CD-3F00-45C6-928B-7954571D8EB7}">
   <dimension ref="A1:Q201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B53" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
@@ -7105,9 +7153,6 @@
       <c r="D5" t="s">
         <v>434</v>
       </c>
-      <c r="F5" t="s">
-        <v>406</v>
-      </c>
       <c r="M5" t="s">
         <v>226</v>
       </c>
@@ -7122,9 +7167,6 @@
       <c r="D6" t="s">
         <v>420</v>
       </c>
-      <c r="F6" t="s">
-        <v>422</v>
-      </c>
       <c r="M6" t="s">
         <v>227</v>
       </c>
@@ -7139,9 +7181,6 @@
       <c r="D7" t="s">
         <v>442</v>
       </c>
-      <c r="F7" t="s">
-        <v>400</v>
-      </c>
       <c r="M7" t="s">
         <v>235</v>
       </c>
@@ -7153,9 +7192,6 @@
       <c r="D8" t="s">
         <v>414</v>
       </c>
-      <c r="F8" t="s">
-        <v>308</v>
-      </c>
       <c r="M8" t="s">
         <v>231</v>
       </c>
@@ -7178,9 +7214,6 @@
       <c r="D10" t="s">
         <v>565</v>
       </c>
-      <c r="F10" t="s">
-        <v>294</v>
-      </c>
       <c r="M10" t="s">
         <v>236</v>
       </c>
@@ -7245,9 +7278,6 @@
       <c r="E15" t="s">
         <v>469</v>
       </c>
-      <c r="F15" t="s">
-        <v>298</v>
-      </c>
       <c r="M15" t="s">
         <v>233</v>
       </c>
@@ -7262,9 +7292,6 @@
       <c r="E16" t="s">
         <v>461</v>
       </c>
-      <c r="F16" t="s">
-        <v>300</v>
-      </c>
       <c r="M16" t="s">
         <v>234</v>
       </c>
@@ -7369,9 +7396,6 @@
       <c r="E26" t="s">
         <v>487</v>
       </c>
-      <c r="F26" t="s">
-        <v>569</v>
-      </c>
       <c r="M26" t="s">
         <v>260</v>
       </c>
@@ -7380,9 +7404,6 @@
       <c r="E27" t="s">
         <v>488</v>
       </c>
-      <c r="F27" t="s">
-        <v>570</v>
-      </c>
       <c r="M27" t="s">
         <v>245</v>
       </c>
@@ -7445,9 +7466,6 @@
       <c r="C34" t="s">
         <v>573</v>
       </c>
-      <c r="F34" t="s">
-        <v>576</v>
-      </c>
       <c r="M34" t="s">
         <v>265</v>
       </c>
@@ -7459,9 +7477,6 @@
       <c r="C35" t="s">
         <v>577</v>
       </c>
-      <c r="F35" t="s">
-        <v>575</v>
-      </c>
       <c r="M35" t="s">
         <v>281</v>
       </c>
@@ -7484,9 +7499,6 @@
       <c r="C37" t="s">
         <v>581</v>
       </c>
-      <c r="F37" t="s">
-        <v>574</v>
-      </c>
       <c r="M37" t="s">
         <v>266</v>
       </c>
@@ -7514,17 +7526,14 @@
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
-        <v>224</v>
-      </c>
-      <c r="F40" t="s">
-        <v>579</v>
-      </c>
       <c r="M40" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
+        <v>513</v>
+      </c>
       <c r="M41" t="s">
         <v>289</v>
       </c>
@@ -7543,11 +7552,11 @@
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D44" t="s">
-        <v>513</v>
+      <c r="E44" t="s">
+        <v>224</v>
       </c>
       <c r="F44" t="s">
-        <v>586</v>
+        <v>298</v>
       </c>
       <c r="M44" t="s">
         <v>202</v>
@@ -7555,7 +7564,7 @@
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
-        <v>587</v>
+        <v>300</v>
       </c>
       <c r="M45" t="s">
         <v>203</v>
@@ -7563,20 +7572,23 @@
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
-        <v>588</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
-        <v>589</v>
+        <v>569</v>
       </c>
       <c r="M47" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="E48" t="s">
+        <v>224</v>
+      </c>
       <c r="F48" t="s">
-        <v>590</v>
+        <v>570</v>
       </c>
       <c r="M48" t="s">
         <v>205</v>
@@ -7595,7 +7607,7 @@
         <v>490</v>
       </c>
       <c r="F50" t="s">
-        <v>592</v>
+        <v>574</v>
       </c>
       <c r="M50" t="s">
         <v>207</v>
@@ -7614,7 +7626,7 @@
         <v>492</v>
       </c>
       <c r="F52" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="M52" t="s">
         <v>208</v>
@@ -7624,11 +7636,8 @@
       <c r="A53" t="s">
         <v>493</v>
       </c>
-      <c r="E53" t="s">
-        <v>224</v>
-      </c>
       <c r="F53" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="M53" t="s">
         <v>209</v>
@@ -7639,7 +7648,7 @@
         <v>494</v>
       </c>
       <c r="F54" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="M54" t="s">
         <v>210</v>
@@ -7649,11 +7658,8 @@
       <c r="A55">
         <v>9512861203</v>
       </c>
-      <c r="E55" t="s">
-        <v>224</v>
-      </c>
       <c r="F55" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="M55" t="s">
         <v>211</v>
@@ -7663,9 +7669,6 @@
       <c r="A56" t="s">
         <v>495</v>
       </c>
-      <c r="F56" t="s">
-        <v>598</v>
-      </c>
       <c r="M56" t="s">
         <v>212</v>
       </c>
@@ -7677,24 +7680,18 @@
       <c r="B57" t="s">
         <v>352</v>
       </c>
-      <c r="E57" t="s">
-        <v>224</v>
-      </c>
-      <c r="F57" t="s">
-        <v>599</v>
-      </c>
       <c r="M57" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
-        <v>600</v>
+        <v>406</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
-        <v>601</v>
+        <v>422</v>
       </c>
       <c r="M59" t="s">
         <v>214</v>
@@ -7702,7 +7699,7 @@
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F60" t="s">
-        <v>602</v>
+        <v>400</v>
       </c>
       <c r="M60" t="s">
         <v>204</v>
@@ -7712,6 +7709,9 @@
       <c r="A61" t="s">
         <v>470</v>
       </c>
+      <c r="F61" t="s">
+        <v>308</v>
+      </c>
       <c r="M61" t="s">
         <v>205</v>
       </c>
@@ -7720,6 +7720,12 @@
       <c r="A62" t="s">
         <v>471</v>
       </c>
+      <c r="E62" t="s">
+        <v>224</v>
+      </c>
+      <c r="F62" t="s">
+        <v>595</v>
+      </c>
       <c r="M62" t="s">
         <v>206</v>
       </c>
@@ -7731,6 +7737,9 @@
       <c r="B63" t="s">
         <v>361</v>
       </c>
+      <c r="F63" t="s">
+        <v>605</v>
+      </c>
       <c r="M63" t="s">
         <v>207</v>
       </c>
@@ -7739,6 +7748,12 @@
       <c r="A64" t="s">
         <v>473</v>
       </c>
+      <c r="D64" t="s">
+        <v>606</v>
+      </c>
+      <c r="F64" t="s">
+        <v>617</v>
+      </c>
       <c r="M64" t="s">
         <v>208</v>
       </c>
@@ -7747,6 +7762,12 @@
       <c r="A65" t="s">
         <v>373</v>
       </c>
+      <c r="D65" t="s">
+        <v>607</v>
+      </c>
+      <c r="F65" t="s">
+        <v>618</v>
+      </c>
       <c r="M65" t="s">
         <v>209</v>
       </c>
@@ -7755,6 +7776,9 @@
       <c r="A66" t="s">
         <v>474</v>
       </c>
+      <c r="D66" t="s">
+        <v>608</v>
+      </c>
       <c r="M66" t="s">
         <v>210</v>
       </c>
@@ -7763,11 +7787,17 @@
       <c r="A67" t="s">
         <v>331</v>
       </c>
+      <c r="D67" t="s">
+        <v>609</v>
+      </c>
       <c r="M67" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D68" t="s">
+        <v>610</v>
+      </c>
       <c r="M68" t="s">
         <v>212</v>
       </c>
@@ -7789,6 +7819,9 @@
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D71" t="s">
+        <v>611</v>
+      </c>
       <c r="M71" t="s">
         <v>221</v>
       </c>
@@ -7797,6 +7830,9 @@
       <c r="A72" t="s">
         <v>503</v>
       </c>
+      <c r="D72" t="s">
+        <v>612</v>
+      </c>
       <c r="M72" t="s">
         <v>225</v>
       </c>
@@ -7805,6 +7841,9 @@
       <c r="A73" t="s">
         <v>504</v>
       </c>
+      <c r="D73" t="s">
+        <v>613</v>
+      </c>
       <c r="M73" t="s">
         <v>226</v>
       </c>
@@ -7813,16 +7852,25 @@
       <c r="A74" t="s">
         <v>505</v>
       </c>
+      <c r="D74" t="s">
+        <v>614</v>
+      </c>
       <c r="M74" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D75" t="s">
+        <v>615</v>
+      </c>
       <c r="M75" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>616</v>
+      </c>
       <c r="M76" t="s">
         <v>255</v>
       </c>
@@ -7837,87 +7885,179 @@
         <v>251</v>
       </c>
     </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E79" t="s">
+        <v>241</v>
+      </c>
+      <c r="F79" t="s">
+        <v>589</v>
+      </c>
+    </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E80" t="s">
+        <v>224</v>
+      </c>
+      <c r="F80" t="s">
+        <v>590</v>
+      </c>
       <c r="M80" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="81" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E81" t="s">
+        <v>241</v>
+      </c>
+      <c r="F81" t="s">
+        <v>603</v>
+      </c>
       <c r="M81" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="82" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E82" t="s">
+        <v>224</v>
+      </c>
+      <c r="F82" t="s">
+        <v>588</v>
+      </c>
       <c r="M82" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="83" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E83" t="s">
+        <v>224</v>
+      </c>
+      <c r="F83" t="s">
+        <v>599</v>
+      </c>
       <c r="M83" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="84" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E84" t="s">
+        <v>224</v>
+      </c>
+      <c r="F84" t="s">
+        <v>597</v>
+      </c>
       <c r="M84" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="85" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E85" t="s">
+        <v>224</v>
+      </c>
+      <c r="F85" t="s">
+        <v>592</v>
+      </c>
       <c r="M85" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="86" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E86" t="s">
+        <v>241</v>
+      </c>
+      <c r="F86" t="s">
+        <v>587</v>
+      </c>
       <c r="M86" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E87" t="s">
+        <v>224</v>
+      </c>
+      <c r="F87" t="s">
+        <v>586</v>
+      </c>
       <c r="M87" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="88" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="88" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E88" t="s">
+        <v>224</v>
+      </c>
+      <c r="F88" t="s">
+        <v>576</v>
+      </c>
       <c r="M88" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="89" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="89" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E89" t="s">
+        <v>224</v>
+      </c>
+      <c r="F89" t="s">
+        <v>575</v>
+      </c>
       <c r="M89" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="90" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="90" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E90" t="s">
+        <v>224</v>
+      </c>
+      <c r="F90" t="s">
+        <v>579</v>
+      </c>
       <c r="M90" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="91" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="91" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E91" t="s">
+        <v>224</v>
+      </c>
+      <c r="F91" t="s">
+        <v>604</v>
+      </c>
       <c r="M91" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="92" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="92" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E92" t="s">
+        <v>224</v>
+      </c>
+      <c r="F92" t="s">
+        <v>594</v>
+      </c>
       <c r="M92" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="93" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="93" spans="5:13" x14ac:dyDescent="0.25">
+      <c r="E93" t="s">
+        <v>224</v>
+      </c>
+      <c r="F93" t="s">
+        <v>600</v>
+      </c>
       <c r="M93" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="94" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="94" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M94" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="95" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="95" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M95" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="96" spans="13:13" x14ac:dyDescent="0.25">
+    <row r="96" spans="5:13" x14ac:dyDescent="0.25">
       <c r="M96" t="s">
         <v>273</v>
       </c>

</xml_diff>